<commit_message>
Automate Update of ChromeDrivers, Restore Locator Files
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -453,11 +453,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45202.45395834765</v>
+        <v>45202.60269819239</v>
       </c>
     </row>
     <row r="3">
@@ -468,11 +468,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45202.45453794114</v>
+        <v>45202.60382008308</v>
       </c>
     </row>
     <row r="4">
@@ -483,11 +483,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45202.45511769969</v>
+        <v>45202.60459474395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring the test cases
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TC_Functional_Smoke_008</t>
+          <t>TC_Functional_Smoke_002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45209.51369260127</v>
+        <v>45217.53852612023</v>
       </c>
     </row>
     <row r="3">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45209.51570525723</v>
+        <v>45217.54047950362</v>
       </c>
     </row>
     <row r="4">
@@ -487,22 +487,112 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45209.51810999016</v>
+        <v>45217.54241007673</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>TC_Functional_Smoke_003</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45217.54501406434</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>TC_Functional_Smoke_008</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>45209.51998262132</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45217.54800098521</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TC_Functional_Smoke_008</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45217.55045021318</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>obj.TC_Functional_Sanity_002_1()</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45217.5552775664</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>obj.TC_Functional_Sanity_002_2()</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45217.56011080815</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>obj.TC_Functional_Sanity_002_3()</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45217.56485854509</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TC_Functional_Smoke_32</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45217.58430443323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>